<commit_message>
Added unit testing, lets a widget connect, and implemented pubsub
</commit_message>
<xml_diff>
--- a/IWC-Mapped Actions.xlsx
+++ b/IWC-Mapped Actions.xlsx
@@ -4,22 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="14355" windowHeight="13860"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="14355" windowHeight="13860" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Legacy" sheetId="1" r:id="rId1"/>
     <sheet name="Container" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Adapter Mapping" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Legacy!$A$1:$E$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Adapter Mapping'!$A$1:$F$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Legacy!$A$1:$F$81</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="142">
   <si>
     <t>names.api</t>
   </si>
@@ -465,12 +467,15 @@
   <si>
     <t>data.api/dashboard/{dashboardId}/widget/{widgetId}/state</t>
   </si>
+  <si>
+    <t>Priority</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,13 +531,35 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -547,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -578,6 +605,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -879,1136 +920,1214 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E156"/>
+  <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A60" sqref="A60"/>
+      <selection pane="bottomRight" activeCell="A45" sqref="A1:F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>139</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>138</v>
       </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" t="s">
         <v>138</v>
       </c>
-      <c r="C7"/>
-      <c r="D7" s="2"/>
-      <c r="E7"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7"/>
+      <c r="E7" s="2"/>
+      <c r="F7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>138</v>
       </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>138</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>138</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>138</v>
       </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>139</v>
       </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>138</v>
       </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="2" t="s">
+      <c r="D15" s="8"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="3">
+        <v>2</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="2" t="s">
+      <c r="D16" s="8"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="3">
+        <v>2</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="2" t="s">
+      <c r="D17" s="8"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="3">
+        <v>2</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="2" t="s">
+      <c r="D18" s="8"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="3">
+        <v>2</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="2" t="s">
+      <c r="D19" s="8"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="3">
+        <v>2</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="2" t="s">
+      <c r="D20" s="8"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="3">
+        <v>2</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="2" t="s">
+      <c r="D21" s="8"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="3">
+        <v>2</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="2" t="s">
+      <c r="D22" s="8"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="3">
+        <v>2</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="2" t="s">
+      <c r="D23" s="8"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="3">
+        <v>2</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="2" t="s">
+      <c r="D24" s="8"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
         <v>99</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>132</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="E25" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>97</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
         <v>99</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>132</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>98</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
         <v>99</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>132</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>78</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>133</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>78</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>134</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>119</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>127</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="D31" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="3">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="3"/>
+      <c r="C33" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="8"/>
+      <c r="E33" s="16"/>
+    </row>
+    <row r="34" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="3"/>
+      <c r="C34" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="7"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="8"/>
+      <c r="E34" s="16"/>
+    </row>
+    <row r="35" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="3"/>
+      <c r="C35" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="8"/>
+      <c r="E35" s="16"/>
+    </row>
+    <row r="36" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="3"/>
+      <c r="C36" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="7"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="8"/>
+      <c r="E36" s="16"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>89</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>89</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>89</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>136</v>
       </c>
-      <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>136</v>
       </c>
-      <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>136</v>
       </c>
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="3">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
         <v>113</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="3">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
         <v>113</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>136</v>
       </c>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>136</v>
       </c>
-      <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="3">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
         <v>115</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>116</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>136</v>
       </c>
-      <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>136</v>
       </c>
-      <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>117</v>
       </c>
-      <c r="D51" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>118</v>
       </c>
-      <c r="D52" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="3">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
         <v>113</v>
       </c>
-      <c r="D53" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E53" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="C54" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>136</v>
       </c>
-      <c r="D55" s="2"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="C56" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="7"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="8"/>
+      <c r="E56" s="7"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="3">
+        <v>3</v>
+      </c>
+      <c r="C57" t="s">
         <v>113</v>
       </c>
-      <c r="D57" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>136</v>
       </c>
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>136</v>
       </c>
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>85</v>
       </c>
-      <c r="D60" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="C61" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C61" s="8"/>
-      <c r="D61" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="8"/>
+      <c r="E61" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="C62" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="C62" s="12"/>
-      <c r="D62" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="12"/>
+      <c r="E62" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="C63" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="8"/>
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="C64" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C64" s="8"/>
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D64" s="8"/>
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" s="3">
+        <v>1</v>
+      </c>
+      <c r="C65" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C65" s="8"/>
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D65" s="8"/>
+      <c r="E65" s="2"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B66" s="3">
+        <v>1</v>
+      </c>
+      <c r="C66" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C66" s="8"/>
-      <c r="D66" s="2"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D66" s="8"/>
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B67" s="3">
+        <v>1</v>
+      </c>
+      <c r="C67" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C67" s="8"/>
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D67" s="8"/>
+      <c r="E67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>140</v>
       </c>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>88</v>
       </c>
-      <c r="D69" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E69" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>140</v>
       </c>
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>87</v>
       </c>
-      <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="C72" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C72" s="8"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="10"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D72" s="8"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="10"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>88</v>
       </c>
-      <c r="D73" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E73" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
         <v>140</v>
       </c>
-      <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>88</v>
       </c>
-      <c r="D75" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E75" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
         <v>140</v>
       </c>
-      <c r="D76" s="2"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
         <v>88</v>
       </c>
-      <c r="D77" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E77" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
         <v>140</v>
       </c>
-      <c r="D78" s="2"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E78" s="2"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>88</v>
       </c>
-      <c r="D79" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E79" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>140</v>
       </c>
-      <c r="D80" s="2"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="2"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>87</v>
       </c>
-      <c r="D81" s="2"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D82" s="2"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="2"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E82" s="2"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>103</v>
       </c>
-      <c r="D83" s="2"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="2"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="C84" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D84" s="2"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="2"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B85" s="8" t="s">
+      <c r="C85" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D85" s="2"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D86" s="2"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D87" s="2"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D88" s="2"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D89" s="2"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D90" s="2"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D91" s="2"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D92" s="2"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D93" s="2"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D94" s="2"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D95" s="2"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D96" s="2"/>
-    </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D97" s="2"/>
-    </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D98" s="2"/>
-    </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D99" s="2"/>
-    </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D100" s="2"/>
-    </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D101" s="2"/>
-    </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D102" s="2"/>
-    </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D103" s="2"/>
-    </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D104" s="2"/>
-    </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D105" s="2"/>
-    </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D106" s="2"/>
-    </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D107" s="2"/>
-    </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D108" s="2"/>
-    </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D109" s="2"/>
-    </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D110" s="2"/>
-    </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D111" s="2"/>
-    </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D112" s="2"/>
-    </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D113" s="2"/>
-    </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D114" s="2"/>
-    </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D115" s="2"/>
-    </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D116" s="2"/>
-    </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D117" s="2"/>
-    </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D118" s="2"/>
-    </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D119" s="2"/>
-    </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D120" s="2"/>
-    </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D121" s="2"/>
-    </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D122" s="2"/>
-    </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D123" s="2"/>
-    </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D124" s="2"/>
-    </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D125" s="2"/>
-    </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D126" s="2"/>
-    </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D127" s="2"/>
-    </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D128" s="2"/>
-    </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D129" s="2"/>
-    </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D130" s="2"/>
-    </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D131" s="2"/>
-    </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D132" s="2"/>
-    </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D133" s="2"/>
-    </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D134" s="2"/>
-    </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D135" s="2"/>
-    </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D136" s="2"/>
-    </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D137" s="2"/>
-    </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D138" s="2"/>
-    </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D139" s="2"/>
-    </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D140" s="2"/>
-    </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D141" s="2"/>
-    </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D142" s="2"/>
-    </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D143" s="2"/>
-    </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D144" s="2"/>
-    </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D145" s="2"/>
-    </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D146" s="2"/>
-    </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D147" s="2"/>
-    </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D148" s="2"/>
-    </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D149" s="2"/>
-    </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D150" s="2"/>
-    </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D151" s="2"/>
-    </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D152" s="2"/>
-    </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D153" s="2"/>
-    </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D154" s="2"/>
-    </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D155" s="2"/>
-    </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D156" s="2"/>
+      <c r="E85" s="2"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E86" s="2"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E87" s="2"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E88" s="2"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E89" s="2"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E90" s="2"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E91" s="2"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E92" s="2"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E93" s="2"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E94" s="2"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E95" s="2"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E96" s="2"/>
+    </row>
+    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E97" s="2"/>
+    </row>
+    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E98" s="2"/>
+    </row>
+    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E99" s="2"/>
+    </row>
+    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E100" s="2"/>
+    </row>
+    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E101" s="2"/>
+    </row>
+    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E102" s="2"/>
+    </row>
+    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E103" s="2"/>
+    </row>
+    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E104" s="2"/>
+    </row>
+    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E105" s="2"/>
+    </row>
+    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E106" s="2"/>
+    </row>
+    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E107" s="2"/>
+    </row>
+    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E108" s="2"/>
+    </row>
+    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E109" s="2"/>
+    </row>
+    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E110" s="2"/>
+    </row>
+    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E111" s="2"/>
+    </row>
+    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E112" s="2"/>
+    </row>
+    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E113" s="2"/>
+    </row>
+    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E114" s="2"/>
+    </row>
+    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E115" s="2"/>
+    </row>
+    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E116" s="2"/>
+    </row>
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E117" s="2"/>
+    </row>
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E118" s="2"/>
+    </row>
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E119" s="2"/>
+    </row>
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E120" s="2"/>
+    </row>
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E121" s="2"/>
+    </row>
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E122" s="2"/>
+    </row>
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E123" s="2"/>
+    </row>
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E124" s="2"/>
+    </row>
+    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E125" s="2"/>
+    </row>
+    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E126" s="2"/>
+    </row>
+    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E127" s="2"/>
+    </row>
+    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E128" s="2"/>
+    </row>
+    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E129" s="2"/>
+    </row>
+    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E130" s="2"/>
+    </row>
+    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E131" s="2"/>
+    </row>
+    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E132" s="2"/>
+    </row>
+    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E133" s="2"/>
+    </row>
+    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E134" s="2"/>
+    </row>
+    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E135" s="2"/>
+    </row>
+    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E136" s="2"/>
+    </row>
+    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E137" s="2"/>
+    </row>
+    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E138" s="2"/>
+    </row>
+    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E139" s="2"/>
+    </row>
+    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E140" s="2"/>
+    </row>
+    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E141" s="2"/>
+    </row>
+    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E142" s="2"/>
+    </row>
+    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E143" s="2"/>
+    </row>
+    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E144" s="2"/>
+    </row>
+    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E145" s="2"/>
+    </row>
+    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E146" s="2"/>
+    </row>
+    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E147" s="2"/>
+    </row>
+    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E148" s="2"/>
+    </row>
+    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E149" s="2"/>
+    </row>
+    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E150" s="2"/>
+    </row>
+    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E151" s="2"/>
+    </row>
+    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E152" s="2"/>
+    </row>
+    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E153" s="2"/>
+    </row>
+    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E154" s="2"/>
+    </row>
+    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E155" s="2"/>
+    </row>
+    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E156" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E81">
+  <autoFilter ref="A1:F81">
     <sortState ref="A2:E81">
       <sortCondition ref="A1:A81"/>
     </sortState>
@@ -2884,4 +3003,1071 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="17"/>
+    </row>
+    <row r="4" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="17"/>
+    </row>
+    <row r="8" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="17"/>
+    </row>
+    <row r="9" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="17"/>
+    </row>
+    <row r="12" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="18">
+        <v>1</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="19"/>
+      <c r="E21" s="20"/>
+    </row>
+    <row r="22" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="18">
+        <v>1</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" s="19"/>
+      <c r="E22" s="20"/>
+    </row>
+    <row r="23" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="18">
+        <v>1</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="3">
+        <v>2</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="3">
+        <v>2</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="3">
+        <v>2</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="3">
+        <v>2</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" t="s">
+        <v>134</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" t="s">
+        <v>127</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="3">
+        <v>2</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D33" s="15"/>
+      <c r="E33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" s="15"/>
+      <c r="E34" s="11"/>
+    </row>
+    <row r="35" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D35" s="15"/>
+      <c r="E35" s="11"/>
+    </row>
+    <row r="36" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D36" s="15"/>
+      <c r="E36" s="11"/>
+    </row>
+    <row r="37" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E40" s="17"/>
+    </row>
+    <row r="41" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E41" s="17"/>
+    </row>
+    <row r="42" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E42" s="17"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="3">
+        <v>2</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43" s="8"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="3">
+        <v>2</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" t="s">
+        <v>136</v>
+      </c>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" t="s">
+        <v>136</v>
+      </c>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="3">
+        <v>2</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" t="s">
+        <v>116</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" t="s">
+        <v>136</v>
+      </c>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" t="s">
+        <v>136</v>
+      </c>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" t="s">
+        <v>117</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" t="s">
+        <v>118</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53" s="3">
+        <v>2</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" s="8"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" t="s">
+        <v>136</v>
+      </c>
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D56" s="8"/>
+      <c r="E56" s="7"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57" s="3">
+        <v>3</v>
+      </c>
+      <c r="C57" t="s">
+        <v>113</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C58" t="s">
+        <v>136</v>
+      </c>
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59" t="s">
+        <v>136</v>
+      </c>
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" t="s">
+        <v>85</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D61" s="8"/>
+      <c r="E61" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D62" s="12"/>
+      <c r="E62" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D63" s="8"/>
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D64" s="8"/>
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B65" s="3">
+        <v>3</v>
+      </c>
+      <c r="C65" t="s">
+        <v>113</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B66" s="3">
+        <v>3</v>
+      </c>
+      <c r="C66" t="s">
+        <v>113</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67" s="3">
+        <v>3</v>
+      </c>
+      <c r="C67" t="s">
+        <v>113</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68" s="3">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>140</v>
+      </c>
+      <c r="E68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" s="3">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s">
+        <v>88</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="3">
+        <v>5</v>
+      </c>
+      <c r="C70" t="s">
+        <v>140</v>
+      </c>
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" t="s">
+        <v>87</v>
+      </c>
+      <c r="E71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D72" s="8"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="10"/>
+    </row>
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73" s="3"/>
+      <c r="C73" t="s">
+        <v>88</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="C74" t="s">
+        <v>140</v>
+      </c>
+      <c r="E74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" t="s">
+        <v>88</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B76" s="3"/>
+      <c r="C76" t="s">
+        <v>140</v>
+      </c>
+      <c r="E76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" t="s">
+        <v>88</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B78" s="3"/>
+      <c r="C78" t="s">
+        <v>140</v>
+      </c>
+      <c r="E78" s="2"/>
+    </row>
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" t="s">
+        <v>88</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B80" s="3"/>
+      <c r="C80" t="s">
+        <v>140</v>
+      </c>
+      <c r="E80" s="2"/>
+    </row>
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B81" s="3"/>
+      <c r="C81" t="s">
+        <v>87</v>
+      </c>
+      <c r="E81" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F81">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="1"/>
+        <filter val="2"/>
+        <filter val="3"/>
+        <filter val="5"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A15:F70">
+      <sortCondition ref="B1:B81"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactored into a listener and participant to allow for multiple owf 7 widgets in the same context
</commit_message>
<xml_diff>
--- a/IWC-Mapped Actions.xlsx
+++ b/IWC-Mapped Actions.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="143">
   <si>
     <t>names.api</t>
   </si>
@@ -469,6 +469,9 @@
   </si>
   <si>
     <t>Priority</t>
+  </si>
+  <si>
+    <t>&lt;&lt;WINDOW.NAME&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -602,9 +605,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -619,6 +619,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1371,7 +1374,7 @@
         <v>135</v>
       </c>
       <c r="D33" s="8"/>
-      <c r="E33" s="16"/>
+      <c r="E33" s="15"/>
     </row>
     <row r="34" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
@@ -1382,7 +1385,7 @@
         <v>135</v>
       </c>
       <c r="D34" s="8"/>
-      <c r="E34" s="16"/>
+      <c r="E34" s="15"/>
     </row>
     <row r="35" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
@@ -1393,7 +1396,7 @@
         <v>135</v>
       </c>
       <c r="D35" s="8"/>
-      <c r="E35" s="16"/>
+      <c r="E35" s="15"/>
     </row>
     <row r="36" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
@@ -1404,7 +1407,7 @@
         <v>135</v>
       </c>
       <c r="D36" s="8"/>
-      <c r="E36" s="16"/>
+      <c r="E36" s="15"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
@@ -2757,10 +2760,10 @@
       <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
     </row>
@@ -3011,7 +3014,7 @@
   <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3045,170 +3048,170 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" s="17"/>
+      <c r="B2" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="17"/>
+      <c r="B3" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="17"/>
+      <c r="B4" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="17"/>
+      <c r="B5" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="17"/>
+      <c r="B6" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E7" s="17"/>
+      <c r="B7" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="16"/>
     </row>
     <row r="8" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="17"/>
+      <c r="B8" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="16"/>
     </row>
     <row r="9" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="17"/>
+      <c r="B9" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="17"/>
+      <c r="B10" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="17"/>
+      <c r="B11" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12" s="17"/>
+      <c r="B12" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="17"/>
+      <c r="B13" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="B14" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="17">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="E15" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="17">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="E16" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="17">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="19" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3251,50 +3254,50 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+    <row r="21" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="17">
         <v>1</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="20"/>
-    </row>
-    <row r="22" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+      <c r="D21" s="18"/>
+      <c r="E21" s="19"/>
+    </row>
+    <row r="22" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="17">
         <v>1</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="20"/>
-    </row>
-    <row r="23" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="D22" s="18"/>
+      <c r="E22" s="19"/>
+    </row>
+    <row r="23" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="17">
         <v>1</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -3438,62 +3441,62 @@
       </c>
     </row>
     <row r="33" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="15" t="s">
+      <c r="B33" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="D33" s="15"/>
+      <c r="D33" s="14"/>
       <c r="E33" s="11"/>
     </row>
     <row r="34" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C34" s="15" t="s">
+      <c r="B34" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="D34" s="15"/>
+      <c r="D34" s="14"/>
       <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="15" t="s">
+      <c r="B35" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="D35" s="15"/>
+      <c r="D35" s="14"/>
       <c r="E35" s="11"/>
     </row>
     <row r="36" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="15" t="s">
+      <c r="B36" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="D36" s="15"/>
+      <c r="D36" s="14"/>
       <c r="E36" s="11"/>
     </row>
     <row r="37" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="13" t="s">
         <v>80</v>
       </c>
       <c r="C37" s="10" t="s">
@@ -3504,10 +3507,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="13" t="s">
         <v>80</v>
       </c>
       <c r="C38" s="10" t="s">
@@ -3518,10 +3521,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="13" t="s">
         <v>80</v>
       </c>
       <c r="C39" s="10" t="s">
@@ -3532,40 +3535,40 @@
       </c>
     </row>
     <row r="40" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="13" t="s">
         <v>80</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="E40" s="17"/>
+      <c r="E40" s="16"/>
     </row>
     <row r="41" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="13" t="s">
         <v>80</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="E41" s="17"/>
+      <c r="E41" s="16"/>
     </row>
     <row r="42" spans="1:6" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="13" t="s">
         <v>80</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="E42" s="17"/>
+      <c r="E42" s="16"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
@@ -3756,7 +3759,7 @@
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>80</v>
@@ -3858,7 +3861,7 @@
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="E65" s="7" t="s">
         <v>80</v>
@@ -3872,7 +3875,7 @@
         <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="E66" s="7" t="s">
         <v>80</v>
@@ -3886,7 +3889,7 @@
         <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="E67" s="7" t="s">
         <v>80</v>
@@ -4069,5 +4072,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>